<commit_message>
Hydroflask E2E Helper,Test data, testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/GoldHydroTestDataE2E.xlsx
+++ b/src/test/resources/TestData/Hydroflask/GoldHydroTestDataE2E.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B896F00-80E0-4211-AE15-ABF8153B3FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F84DD94-57C1-4D08-8C71-943442BDF011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19170" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="144">
   <si>
     <t>UserName</t>
   </si>
@@ -452,6 +452,12 @@
   </si>
   <si>
     <t>Every experience is a story no one else can tell, including every sticker, bump, ding and mark along the way.</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -816,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,6 +1107,9 @@
       <c r="A15" t="s">
         <v>37</v>
       </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
       <c r="P15" s="5" t="s">
         <v>38</v>
       </c>
@@ -1333,10 +1342,10 @@
         <v>122</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="W29" t="s">
         <v>141</v>

</xml_diff>